<commit_message>
Seventh day - dictionaty improvements
</commit_message>
<xml_diff>
--- a/teste-excelnew-teste-traduzido.xlsx
+++ b/teste-excelnew-teste-traduzido.xlsx
@@ -453,7 +453,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE ÁREAS ISOLADAS NORTE </t>
+          <t>SAIN</t>
         </is>
       </c>
     </row>
@@ -477,7 +477,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE MÚLTIPLAS ATIVIDADES SUL </t>
+          <t>SMAS</t>
         </is>
       </c>
     </row>
@@ -489,7 +489,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE HABITAÇÕES INDIVIDUAIS SUL </t>
+          <t>SHIS</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE DIVERSÕES NORTE </t>
+          <t>SDN</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE ADMINISTRAÇÃO MUNICIPAL </t>
+          <t>SAM</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR MÉDICO HOSPITALAR SUL </t>
+          <t>SMHS</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>SETOR DE EMBAIXADAS NORTE</t>
+          <t>SEN</t>
         </is>
       </c>
     </row>
@@ -573,7 +573,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>SETOR DE HABITAÇÕES COLETIVAS NOROESTE</t>
+          <t>SHCNW</t>
         </is>
       </c>
     </row>
@@ -621,7 +621,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t xml:space="preserve">ÁREA DE EXPANSÃO DOS MINISTÉRIOS NORTE </t>
+          <t>AEMN</t>
         </is>
       </c>
     </row>
@@ -633,7 +633,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ÁREA DE DESENVOLVIMENTO ECONÔMICO</t>
+          <t>ADE</t>
         </is>
       </c>
     </row>
@@ -669,7 +669,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>SETOR HABITACIONAL COLETIVAS GEMINADAS NORTE</t>
+          <t>SHCGN</t>
         </is>
       </c>
     </row>
@@ -681,7 +681,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR BANCÁRIO NORTE </t>
+          <t>SBN</t>
         </is>
       </c>
     </row>
@@ -693,7 +693,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE MÚLTIPLAS ATIVIDADES SUL </t>
+          <t>SMAS</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE CLUBES ESPORTIVOS NORTE </t>
+          <t>SCEN</t>
         </is>
       </c>
     </row>
@@ -741,7 +741,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE ÁREAS ISOLADAS SUDOESTE </t>
+          <t>SAI/SO</t>
         </is>
       </c>
     </row>
@@ -765,7 +765,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t xml:space="preserve">ESPLANADA DOS MINISTÉRIOS </t>
+          <t>EMI</t>
         </is>
       </c>
     </row>
@@ -777,7 +777,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE EDIFÍCIOS PÚBLICOS SUL </t>
+          <t>SEPS</t>
         </is>
       </c>
     </row>
@@ -789,7 +789,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE GRANDES ÁREAS SUL </t>
+          <t>SGAS</t>
         </is>
       </c>
     </row>
@@ -801,7 +801,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE ÁREAS ISOLADAS NORTE </t>
+          <t>SAIN</t>
         </is>
       </c>
     </row>
@@ -837,7 +837,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>SETOR HOTELEIRO SUL</t>
+          <t>SHS</t>
         </is>
       </c>
     </row>
@@ -849,7 +849,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR HOSPITALAR LOCAL SUDOESTE </t>
+          <t>SHLSW</t>
         </is>
       </c>
     </row>
@@ -897,7 +897,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>SETOR POLICIAL</t>
+          <t>SPO</t>
         </is>
       </c>
     </row>
@@ -933,7 +933,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>SETOR DE GARAGENS E CONCESSIONÁRIAS DE VEÍCULOS - NORTE E SUL</t>
+          <t>SGCV</t>
         </is>
       </c>
     </row>
@@ -945,7 +945,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR MILITAR URBANO </t>
+          <t>SMU</t>
         </is>
       </c>
     </row>
@@ -1005,7 +1005,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>SETOR HOSPITALAR LOCAL SUL</t>
+          <t>SHLS</t>
         </is>
       </c>
     </row>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR BANCÁRIO SUL </t>
+          <t>SBS</t>
         </is>
       </c>
     </row>
@@ -1029,7 +1029,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE RÁDIO E TELEVISÃO NORTE </t>
+          <t>SRTVN</t>
         </is>
       </c>
     </row>
@@ -1053,7 +1053,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE INDÚSTRIAS GRÁFICAS </t>
+          <t>SIG</t>
         </is>
       </c>
     </row>
@@ -1065,7 +1065,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>SETOR DE DIVULGAÇÃO CULTURAL</t>
+          <t>SDC</t>
         </is>
       </c>
     </row>
@@ -1077,7 +1077,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE ÁREAS ISOLADAS NORTE </t>
+          <t>SAIN</t>
         </is>
       </c>
     </row>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>SETOR HABITACIONAL COLETIVAS GEMINADAS NORTE</t>
+          <t>SHCGN</t>
         </is>
       </c>
     </row>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>SETOR HABITACIONAL COLETIVAS GEMINADAS NORTE</t>
+          <t>SHCGN</t>
         </is>
       </c>
     </row>
@@ -1137,7 +1137,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE DIVERSÕES SUL </t>
+          <t>SDS</t>
         </is>
       </c>
     </row>
@@ -1245,7 +1245,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>SETOR TERMINAL NORTE - REGIÃO DO BOULEVARD SHOPPING</t>
+          <t>STN</t>
         </is>
       </c>
     </row>
@@ -1293,7 +1293,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE RÁDIO E TELEVISÃO SUL </t>
+          <t>SRTVS</t>
         </is>
       </c>
     </row>
@@ -1305,7 +1305,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE ÁREAS ISOLADAS SUL </t>
+          <t>SAIS</t>
         </is>
       </c>
     </row>
@@ -1317,7 +1317,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE ÁREAS ISOLADAS NORTE </t>
+          <t>SAIN</t>
         </is>
       </c>
     </row>
@@ -1329,7 +1329,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>SETOR CULTURAL SUL</t>
+          <t>SCTS</t>
         </is>
       </c>
     </row>
@@ -1341,7 +1341,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>SETOR TERMINAL SUL</t>
+          <t>STS</t>
         </is>
       </c>
     </row>
@@ -1365,7 +1365,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE ÁREAS ISOLADAS SUL </t>
+          <t>SAIS</t>
         </is>
       </c>
     </row>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>SETOR COMERCIAL LOCAL NORTE</t>
+          <t>SCLN</t>
         </is>
       </c>
     </row>
@@ -1389,7 +1389,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>SETOR DE RECREATIVO E PARQUES SUL - PARQUE DA CIDADE</t>
+          <t>SRPS</t>
         </is>
       </c>
     </row>
@@ -1425,7 +1425,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>SETOR HABITACIONAL COLETIVAS GEMINADAS NORTE</t>
+          <t>SHCGN</t>
         </is>
       </c>
     </row>
@@ -1437,7 +1437,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>PLATAFORMA RODOVIÁRIA</t>
+          <t>PFR</t>
         </is>
       </c>
     </row>
@@ -1525,7 +1525,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>EIXO MONUMENTAL</t>
+          <t>EMO</t>
         </is>
       </c>
     </row>
@@ -1549,7 +1549,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE ÁREAS ISOLADAS SUL </t>
+          <t>SAIS</t>
         </is>
       </c>
     </row>
@@ -1609,7 +1609,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE ÁREAS ISOLADAS SUL </t>
+          <t>SAIS</t>
         </is>
       </c>
     </row>
@@ -1705,7 +1705,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE ÁREAS ISOLADAS NORTE </t>
+          <t>SAIN</t>
         </is>
       </c>
     </row>
@@ -1753,7 +1753,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR PALÁCIO PRESIDENCIAL </t>
+          <t>SPP</t>
         </is>
       </c>
     </row>
@@ -1801,7 +1801,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE ÁREAS ISOLADAS SUL </t>
+          <t>SAIS</t>
         </is>
       </c>
     </row>
@@ -1849,7 +1849,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>SETOR DE CLUBES ESPORTIVOS SUL</t>
+          <t>SCES</t>
         </is>
       </c>
     </row>
@@ -1861,7 +1861,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>SETOR ERMIDA DOM BOSCO</t>
+          <t>SEDB</t>
         </is>
       </c>
     </row>
@@ -1993,7 +1993,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE ÁREAS ISOLADAS SUDOESTE </t>
+          <t>SAI/SO</t>
         </is>
       </c>
     </row>
@@ -2005,7 +2005,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE ÁREAS ISOLADAS NORTE </t>
+          <t>SAIN</t>
         </is>
       </c>
     </row>
@@ -2029,7 +2029,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>PRAÇA DOS TRÊS PODERES</t>
+          <t>PTP</t>
         </is>
       </c>
     </row>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE ADMINISTRAÇÃO FEDERAL NORTE </t>
+          <t>SAFN</t>
         </is>
       </c>
     </row>
@@ -2089,7 +2089,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>SETOR HABITACIONAL COLETIVAS GEMINADAS NORTE</t>
+          <t>SHCGN</t>
         </is>
       </c>
     </row>
@@ -2101,7 +2101,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE HABITAÇÕES COLETIVAS ECONÔMICAS SUL - CRUZEIRO NOVO </t>
+          <t>SHCES</t>
         </is>
       </c>
     </row>
@@ -2137,7 +2137,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE HABITAÇÕES INDIVIDUAIS NORTE </t>
+          <t>SHIN</t>
         </is>
       </c>
     </row>
@@ -2149,7 +2149,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>SETOR HABITACIONAL COLETIVAS GEMINADAS NORTE</t>
+          <t>SHCGN</t>
         </is>
       </c>
     </row>
@@ -2209,7 +2209,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR MÉDICO HOSPITALAR NORTE </t>
+          <t>SMHN</t>
         </is>
       </c>
     </row>
@@ -2221,7 +2221,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR COMPLEMENTAR DE INDÚSTRIA E ABASTECIMENTO </t>
+          <t>SCIA</t>
         </is>
       </c>
     </row>
@@ -2233,7 +2233,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE MANSÕES DOM BOSCO </t>
+          <t>SMDB</t>
         </is>
       </c>
     </row>
@@ -2245,7 +2245,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>SETOR DE POSTOS E MOTEIS</t>
+          <t>SPMN</t>
         </is>
       </c>
     </row>
@@ -2317,7 +2317,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>SETOR HABITACIONAL COLETIVAS GEMINADAS NORTE</t>
+          <t>SHCGN</t>
         </is>
       </c>
     </row>
@@ -2365,7 +2365,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>ÁREA DE DESENVOLVIMENTO ECONÔMICO</t>
+          <t>ADE</t>
         </is>
       </c>
     </row>
@@ -2377,7 +2377,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>SETOR DE MATERIAIS DE CONSTRUÇÃO - CEILÂNDIA</t>
+          <t>SDMC</t>
         </is>
       </c>
     </row>
@@ -2413,7 +2413,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>QUADRAS ECONÔMICAS LÚCIO COSTA  - GUARÁ</t>
+          <t>QELC</t>
         </is>
       </c>
     </row>
@@ -2473,7 +2473,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR COMERCIAL LOCAL RESIDENCIAL NORTE </t>
+          <t>SCLRN</t>
         </is>
       </c>
     </row>
@@ -2521,7 +2521,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE EDIFÍCIOS PÚBLICOS NORTE </t>
+          <t>SEPN</t>
         </is>
       </c>
     </row>
@@ -2569,7 +2569,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>VILA PLANALTO</t>
+          <t>VPLA</t>
         </is>
       </c>
     </row>
@@ -2581,7 +2581,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE INDÚSTRIA E ABASTECIMENTO </t>
+          <t>SIA</t>
         </is>
       </c>
     </row>
@@ -2617,7 +2617,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>SETOR DE RESIDÊNCIAS ECONÔMICAS SUL - CRUZEIRO VELHO</t>
+          <t>SRES</t>
         </is>
       </c>
     </row>
@@ -2629,7 +2629,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE TRANSPORTE REGIONAL DE CARGAS </t>
+          <t>STRC</t>
         </is>
       </c>
     </row>
@@ -2689,7 +2689,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE ÁREAS ISOLADAS SUDOESTE </t>
+          <t>SAI/SO</t>
         </is>
       </c>
     </row>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>SETOR HABITACIONAL TAQUARI - LAGO NORTE</t>
+          <t>SHTQ</t>
         </is>
       </c>
     </row>
@@ -2821,7 +2821,7 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>ÁREA DE DESENVOLVIMENTO ECONÔMICO</t>
+          <t>ADE</t>
         </is>
       </c>
     </row>
@@ -2857,7 +2857,7 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR HOSPITALAR LOCAL NORTE </t>
+          <t>SHLN</t>
         </is>
       </c>
     </row>
@@ -2953,7 +2953,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>SETOR DE PRESERVAÇÃO DA VILA PLANALTO</t>
+          <t>SPVP</t>
         </is>
       </c>
     </row>
@@ -3001,7 +3001,7 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE EMBAIXADAS SUL </t>
+          <t>SES</t>
         </is>
       </c>
     </row>
@@ -3013,7 +3013,7 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE GRANDES ÁREAS NORTE </t>
+          <t>SGAN</t>
         </is>
       </c>
     </row>
@@ -3061,7 +3061,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>SETOR HOTELEIRO NORTE</t>
+          <t>SHN</t>
         </is>
       </c>
     </row>
@@ -3073,7 +3073,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>EIXO RODOVIÁRIO NORTE</t>
+          <t>ERN</t>
         </is>
       </c>
     </row>
@@ -3121,7 +3121,7 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE ÁREAS ISOLADAS SUL </t>
+          <t>SAIS</t>
         </is>
       </c>
     </row>
@@ -3133,7 +3133,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>SETOR DE GARAGENS DOS MINISTÉRIOS NORTE</t>
+          <t>SGMN</t>
         </is>
       </c>
     </row>
@@ -3145,7 +3145,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE CLUBES ESPORTIVOS NORTE </t>
+          <t>SCEN</t>
         </is>
       </c>
     </row>
@@ -3181,7 +3181,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR CULTURAL NORTE  - TEATRO NACIONAL </t>
+          <t>SCTN</t>
         </is>
       </c>
     </row>
@@ -3193,7 +3193,7 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>EIXO RODOVIÁRIO SUL</t>
+          <t>ERS</t>
         </is>
       </c>
     </row>
@@ -3229,7 +3229,7 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE GRANDES ÁREAS NORTE </t>
+          <t>SGAN</t>
         </is>
       </c>
     </row>
@@ -3241,7 +3241,7 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE GRANDES ÁREAS SUL </t>
+          <t>SGAS</t>
         </is>
       </c>
     </row>
@@ -3289,7 +3289,7 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>SETOR DE HABITAÇÕES INDIVIDUAIS GEMINADAS SUL</t>
+          <t>SHIGS</t>
         </is>
       </c>
     </row>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE ÁREAS ISOLADAS NORTE </t>
+          <t>SAIN</t>
         </is>
       </c>
     </row>
@@ -3325,7 +3325,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE HOTÉIS E TURISMO NORTE </t>
+          <t>SHTN</t>
         </is>
       </c>
     </row>
@@ -3337,7 +3337,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>SETOR COMERCIAL RESIDENCIAL NORTE</t>
+          <t>SCRN</t>
         </is>
       </c>
     </row>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>SETOR COMERCIAL LOCAL NORTE</t>
+          <t>SCLN</t>
         </is>
       </c>
     </row>
@@ -3361,7 +3361,7 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE HABITAÇÕES COLETIVAS SUDOESTE </t>
+          <t>SHCSW</t>
         </is>
       </c>
     </row>
@@ -3373,7 +3373,7 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>SETOR DE CLUBES ESPORTIVOS SUL</t>
+          <t>SCES</t>
         </is>
       </c>
     </row>
@@ -3385,7 +3385,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR COMERCIAL SUL </t>
+          <t>SCS</t>
         </is>
       </c>
     </row>
@@ -3397,7 +3397,7 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>PRAÇA MUNICIPAL</t>
+          <t>PMU</t>
         </is>
       </c>
     </row>
@@ -3409,7 +3409,7 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE ÁREAS ISOLADAS SUL </t>
+          <t>SAIS</t>
         </is>
       </c>
     </row>
@@ -3421,7 +3421,7 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>SETOR COMERCIAL RESIDENCIAL SUL</t>
+          <t>SCRS</t>
         </is>
       </c>
     </row>
@@ -3433,7 +3433,7 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>SETOR COMERCIAL LOCAL SUL</t>
+          <t>SCLS</t>
         </is>
       </c>
     </row>
@@ -3445,7 +3445,7 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>SETOR COMERCIAL LOCAL SUL</t>
+          <t>SCLS</t>
         </is>
       </c>
     </row>
@@ -3457,7 +3457,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>SETOR HOSPITALAR PÚBLICO DE BRASÍLIA</t>
+          <t>SHPB</t>
         </is>
       </c>
     </row>
@@ -3601,7 +3601,7 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE ADMINISTRAÇÃO FEDERAL SUL </t>
+          <t>SAFS</t>
         </is>
       </c>
     </row>
@@ -3625,7 +3625,7 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>SETOR HABITACIONAL ARNIQUEIRAS</t>
+          <t>SHA</t>
         </is>
       </c>
     </row>
@@ -3673,7 +3673,7 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>SETOR HABITACIONAL ARNIQUEIRAS</t>
+          <t>SHA</t>
         </is>
       </c>
     </row>
@@ -3779,7 +3779,11 @@
           <t>SHJK</t>
         </is>
       </c>
-      <c r="B280" t="inlineStr"/>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>SHJK</t>
+        </is>
+      </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
@@ -3933,7 +3937,7 @@
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t xml:space="preserve">SETOR DE ÁREAS ISOLADAS SUL </t>
+          <t>SAIS</t>
         </is>
       </c>
     </row>

</xml_diff>